<commit_message>
fixed north vancouver city/district description
</commit_message>
<xml_diff>
--- a/2014-vancouver-cts-matched-to-munis/Vancouver-CTs-Matched-to-Munis.xlsx
+++ b/2014-vancouver-cts-matched-to-munis/Vancouver-CTs-Matched-to-Munis.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Vancouver CTs Matched to CSDs -" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Vancouver CTs Matched to CSDs -'!$A$1:$F$458</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="122">
   <si>
     <t>CTUID</t>
   </si>
@@ -374,6 +377,12 @@
   </si>
   <si>
     <t>9330150.00</t>
+  </si>
+  <si>
+    <t>North Vancovuer District</t>
+  </si>
+  <si>
+    <t>North Vancouver City</t>
   </si>
 </sst>
 </file>
@@ -1206,7 +1215,7 @@
   <dimension ref="A1:E458"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1336,7 @@
         <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -1429,7 +1438,7 @@
         <v>9330100.0099999998</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -1633,7 +1642,7 @@
         <v>9330111.0299999993</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -1667,7 +1676,7 @@
         <v>9330101.0399999991</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -1973,7 +1982,7 @@
         <v>9330114.0199999996</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -2211,7 +2220,7 @@
         <v>9330111.0199999996</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -2483,7 +2492,7 @@
         <v>51</v>
       </c>
       <c r="C75" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D75" t="s">
         <v>11</v>
@@ -2500,7 +2509,7 @@
         <v>52</v>
       </c>
       <c r="C76" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D76" t="s">
         <v>11</v>
@@ -2670,7 +2679,7 @@
         <v>9330110.0199999996</v>
       </c>
       <c r="C86" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D86" t="s">
         <v>11</v>
@@ -3605,7 +3614,7 @@
         <v>61</v>
       </c>
       <c r="C141" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D141" t="s">
         <v>11</v>
@@ -3826,7 +3835,7 @@
         <v>9330111.0099999998</v>
       </c>
       <c r="C154" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D154" t="s">
         <v>11</v>
@@ -3843,7 +3852,7 @@
         <v>9330101.0299999993</v>
       </c>
       <c r="C155" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D155" t="s">
         <v>11</v>
@@ -3962,7 +3971,7 @@
         <v>64</v>
       </c>
       <c r="C162" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D162" t="s">
         <v>11</v>
@@ -4047,7 +4056,7 @@
         <v>66</v>
       </c>
       <c r="C167" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D167" t="s">
         <v>11</v>
@@ -4234,7 +4243,7 @@
         <v>9330101.0500000007</v>
       </c>
       <c r="C178" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D178" t="s">
         <v>11</v>
@@ -4727,7 +4736,7 @@
         <v>9330101.0600000005</v>
       </c>
       <c r="C207" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D207" t="s">
         <v>11</v>
@@ -4880,7 +4889,7 @@
         <v>9330100.0199999996</v>
       </c>
       <c r="C216" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D216" t="s">
         <v>11</v>
@@ -4965,7 +4974,7 @@
         <v>73</v>
       </c>
       <c r="C221" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D221" t="s">
         <v>11</v>
@@ -5016,7 +5025,7 @@
         <v>74</v>
       </c>
       <c r="C224" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D224" t="s">
         <v>11</v>
@@ -5050,7 +5059,7 @@
         <v>75</v>
       </c>
       <c r="C226" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D226" t="s">
         <v>11</v>
@@ -5390,7 +5399,7 @@
         <v>9330114.0099999998</v>
       </c>
       <c r="C246" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D246" t="s">
         <v>11</v>
@@ -6087,7 +6096,7 @@
         <v>85</v>
       </c>
       <c r="C287" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D287" t="s">
         <v>11</v>
@@ -6478,7 +6487,7 @@
         <v>9330110.0399999991</v>
       </c>
       <c r="C310" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D310" t="s">
         <v>11</v>
@@ -7005,7 +7014,7 @@
         <v>9330110.0299999993</v>
       </c>
       <c r="C341" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D341" t="s">
         <v>11</v>
@@ -7498,7 +7507,7 @@
         <v>104</v>
       </c>
       <c r="C370" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D370" t="s">
         <v>11</v>
@@ -8025,7 +8034,7 @@
         <v>110</v>
       </c>
       <c r="C401" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D401" t="s">
         <v>11</v>
@@ -8348,7 +8357,7 @@
         <v>113</v>
       </c>
       <c r="C420" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="D420" t="s">
         <v>11</v>

</xml_diff>